<commit_message>
Fix : Excel SO파일 생성 문제
불러올 때 이름 차이로 인한 할당 문제 발생  -> Rename 해결
</commit_message>
<xml_diff>
--- a/Survival/Assets/Excel/BuildItemData.xlsx
+++ b/Survival/Assets/Excel/BuildItemData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajin\Desktop\Unity\Unity_project\TeamProject_Survival\Survival\Survival\Assets\Resources\DataSO\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajin\Desktop\Unity\Unity_project\TeamProject_Survival\Survival\Survival\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FCB87-4CA1-4742-A206-2BBFAE058C67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA9017-E57E-4537-BDC3-6FC870376CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10128" yWindow="1956" windowWidth="20796" windowHeight="12120" xr2:uid="{87CC9680-1ADE-4891-8706-9F68FAE83D61}"/>
+    <workbookView xWindow="-22980" yWindow="0" windowWidth="23040" windowHeight="12120" xr2:uid="{87CC9680-1ADE-4891-8706-9F68FAE83D61}"/>
   </bookViews>
   <sheets>
     <sheet name="BuildItem" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +103,14 @@
   </si>
   <si>
     <t>나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite/well</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/well</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -490,7 +498,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -500,7 +508,8 @@
     <col min="5" max="5" width="16.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
@@ -554,6 +563,12 @@
       <c r="G2">
         <v>20</v>
       </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3">
@@ -577,6 +592,12 @@
       <c r="G3">
         <v>10</v>
       </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4">
@@ -599,6 +620,12 @@
       </c>
       <c r="G4">
         <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>